<commit_message>
update with final results
Update avec les fichiers proclamés par le CC
</commit_message>
<xml_diff>
--- a/data/P2022_Resultats_Régions_T1.xlsx
+++ b/data/P2022_Resultats_Régions_T1.xlsx
@@ -773,154 +773,154 @@
         <v>53</v>
       </c>
       <c r="C2" t="n">
-        <v>3862884</v>
+        <v>3862920</v>
       </c>
       <c r="D2" t="n">
-        <v>1008217</v>
+        <v>1008344</v>
       </c>
       <c r="E2" t="n">
-        <v>26.1001106944967</v>
+        <v>26.103155126174</v>
       </c>
       <c r="F2" t="n">
-        <v>2854667</v>
+        <v>2854576</v>
       </c>
       <c r="G2" t="n">
-        <v>73.8998893055034</v>
+        <v>73.896844873826</v>
       </c>
       <c r="H2" t="n">
-        <v>42182</v>
+        <v>42255</v>
       </c>
       <c r="I2" t="n">
-        <v>1.0919820527875</v>
+        <v>1.09386163834612</v>
       </c>
       <c r="J2" t="n">
-        <v>1.47765045800438</v>
+        <v>1.48025486096709</v>
       </c>
       <c r="K2" t="n">
-        <v>18665</v>
+        <v>18647</v>
       </c>
       <c r="L2" t="n">
-        <v>0.483188208602692</v>
+        <v>0.48271773684156</v>
       </c>
       <c r="M2" t="n">
-        <v>0.653841586426718</v>
+        <v>0.653231863506174</v>
       </c>
       <c r="N2" t="n">
-        <v>2793820</v>
+        <v>2793674</v>
       </c>
       <c r="O2" t="n">
-        <v>72.3247190441132</v>
+        <v>72.3202654986383</v>
       </c>
       <c r="P2" t="n">
-        <v>97.8685079555689</v>
+        <v>97.8665132755267</v>
       </c>
       <c r="Q2" t="n">
-        <v>18658</v>
+        <v>18655</v>
       </c>
       <c r="R2" t="n">
         <v>47422</v>
       </c>
       <c r="S2" t="n">
-        <v>762259</v>
+        <v>762241</v>
       </c>
       <c r="T2" t="n">
-        <v>77453</v>
+        <v>77439</v>
       </c>
       <c r="U2" t="n">
-        <v>825215</v>
+        <v>825196</v>
       </c>
       <c r="V2" t="n">
-        <v>200289</v>
+        <v>200256</v>
       </c>
       <c r="W2" t="n">
-        <v>492448</v>
+        <v>492408</v>
       </c>
       <c r="X2" t="n">
-        <v>40032</v>
+        <v>40030</v>
       </c>
       <c r="Y2" t="n">
-        <v>111974</v>
+        <v>111953</v>
       </c>
       <c r="Z2" t="n">
-        <v>120914</v>
+        <v>120917</v>
       </c>
       <c r="AA2" t="n">
-        <v>22240</v>
+        <v>22241</v>
       </c>
       <c r="AB2" t="n">
         <v>74916</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.483006996844844</v>
+        <v>0.482924834063351</v>
       </c>
       <c r="AD2" t="n">
-        <v>1.22763199723316</v>
+        <v>1.22762055647023</v>
       </c>
       <c r="AE2" t="n">
-        <v>19.732899046412</v>
+        <v>19.7322491793773</v>
       </c>
       <c r="AF2" t="n">
-        <v>2.00505632579182</v>
+        <v>2.00467521978193</v>
       </c>
       <c r="AG2" t="n">
-        <v>21.3626658217021</v>
+        <v>21.361974879107</v>
       </c>
       <c r="AH2" t="n">
-        <v>5.18496025249529</v>
+        <v>5.18405765586655</v>
       </c>
       <c r="AI2" t="n">
-        <v>12.7481953897658</v>
+        <v>12.7470410984437</v>
       </c>
       <c r="AJ2" t="n">
-        <v>1.03632415573442</v>
+        <v>1.03626272353556</v>
       </c>
       <c r="AK2" t="n">
-        <v>2.8987150533125</v>
+        <v>2.89814440889275</v>
       </c>
       <c r="AL2" t="n">
-        <v>3.13014835547741</v>
+        <v>3.13019684590931</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.575735642074678</v>
+        <v>0.575756163731064</v>
       </c>
       <c r="AN2" t="n">
-        <v>1.93938000726918</v>
+        <v>1.93936193345966</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.667831141591083</v>
+        <v>0.667758657595697</v>
       </c>
       <c r="AP2" t="n">
-        <v>1.69738923767458</v>
+        <v>1.69747794481389</v>
       </c>
       <c r="AQ2" t="n">
-        <v>27.2837548589387</v>
+        <v>27.2845364204986</v>
       </c>
       <c r="AR2" t="n">
-        <v>2.77229742789442</v>
+        <v>2.77194117853407</v>
       </c>
       <c r="AS2" t="n">
-        <v>29.537157010831</v>
+        <v>29.5380205421248</v>
       </c>
       <c r="AT2" t="n">
-        <v>7.16900158206327</v>
+        <v>7.16819500056198</v>
       </c>
       <c r="AU2" t="n">
-        <v>17.6263324050941</v>
+        <v>17.6258217673215</v>
       </c>
       <c r="AV2" t="n">
-        <v>1.43287684961809</v>
+        <v>1.43288014277972</v>
       </c>
       <c r="AW2" t="n">
-        <v>4.00791747499839</v>
+        <v>4.00737523418982</v>
       </c>
       <c r="AX2" t="n">
-        <v>4.32790945730219</v>
+        <v>4.32824302334489</v>
       </c>
       <c r="AY2" t="n">
-        <v>0.79604269423227</v>
+        <v>0.796120091320605</v>
       </c>
       <c r="AZ2" t="n">
-        <v>2.6814898597619</v>
+        <v>2.68162999691446</v>
       </c>
     </row>
     <row r="3">
@@ -931,154 +931,154 @@
         <v>55</v>
       </c>
       <c r="C3" t="n">
-        <v>4463031</v>
+        <v>4463041</v>
       </c>
       <c r="D3" t="n">
-        <v>962488</v>
+        <v>962499</v>
       </c>
       <c r="E3" t="n">
-        <v>21.5657923953475</v>
+        <v>21.5659905432193</v>
       </c>
       <c r="F3" t="n">
-        <v>3500543</v>
+        <v>3500542</v>
       </c>
       <c r="G3" t="n">
-        <v>78.4342076046525</v>
+        <v>78.4340094567807</v>
       </c>
       <c r="H3" t="n">
-        <v>53355</v>
+        <v>53440</v>
       </c>
       <c r="I3" t="n">
-        <v>1.19548799907507</v>
+        <v>1.19738985144882</v>
       </c>
       <c r="J3" t="n">
-        <v>1.52419210391074</v>
+        <v>1.52662073473194</v>
       </c>
       <c r="K3" t="n">
-        <v>26378</v>
+        <v>27129</v>
       </c>
       <c r="L3" t="n">
-        <v>0.591033313458947</v>
+        <v>0.607859080837483</v>
       </c>
       <c r="M3" t="n">
-        <v>0.753540236471885</v>
+        <v>0.774994272315544</v>
       </c>
       <c r="N3" t="n">
-        <v>3420810</v>
+        <v>3419973</v>
       </c>
       <c r="O3" t="n">
-        <v>76.6476862921185</v>
+        <v>76.6287605244944</v>
       </c>
       <c r="P3" t="n">
-        <v>97.7222676596174</v>
+        <v>97.6983849929525</v>
       </c>
       <c r="Q3" t="n">
-        <v>18497</v>
+        <v>18494</v>
       </c>
       <c r="R3" t="n">
-        <v>96800</v>
+        <v>96771</v>
       </c>
       <c r="S3" t="n">
-        <v>945330</v>
+        <v>945122</v>
       </c>
       <c r="T3" t="n">
-        <v>201771</v>
+        <v>201726</v>
       </c>
       <c r="U3" t="n">
-        <v>779945</v>
+        <v>779699</v>
       </c>
       <c r="V3" t="n">
-        <v>210501</v>
+        <v>210476</v>
       </c>
       <c r="W3" t="n">
-        <v>681405</v>
+        <v>681218</v>
       </c>
       <c r="X3" t="n">
-        <v>77326</v>
+        <v>77306</v>
       </c>
       <c r="Y3" t="n">
-        <v>151746</v>
+        <v>151714</v>
       </c>
       <c r="Z3" t="n">
-        <v>157229</v>
+        <v>157205</v>
       </c>
       <c r="AA3" t="n">
-        <v>32598</v>
+        <v>32597</v>
       </c>
       <c r="AB3" t="n">
-        <v>67662</v>
+        <v>67645</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.414449283457812</v>
+        <v>0.41438113609084</v>
       </c>
       <c r="AD3" t="n">
-        <v>2.16892959067504</v>
+        <v>2.16827494974839</v>
       </c>
       <c r="AE3" t="n">
-        <v>21.1813451441408</v>
+        <v>21.1766371852734</v>
       </c>
       <c r="AF3" t="n">
-        <v>4.52094103760427</v>
+        <v>4.5199226267471</v>
       </c>
       <c r="AG3" t="n">
-        <v>17.4756796446182</v>
+        <v>17.4701285513622</v>
       </c>
       <c r="AH3" t="n">
-        <v>4.71654801411866</v>
+        <v>4.71597728992407</v>
       </c>
       <c r="AI3" t="n">
-        <v>15.2677630964248</v>
+        <v>15.2635389188672</v>
       </c>
       <c r="AJ3" t="n">
-        <v>1.73258935463366</v>
+        <v>1.73213734760671</v>
       </c>
       <c r="AK3" t="n">
-        <v>3.40006600895221</v>
+        <v>3.39934139076921</v>
       </c>
       <c r="AL3" t="n">
-        <v>3.52291973772981</v>
+        <v>3.52237409425546</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.730400483438273</v>
+        <v>0.730376440637673</v>
       </c>
       <c r="AN3" t="n">
-        <v>1.51605489632494</v>
+        <v>1.51567059321212</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.540719887979747</v>
+        <v>0.540764503111574</v>
       </c>
       <c r="AP3" t="n">
-        <v>2.82973915534625</v>
+        <v>2.82958374232779</v>
       </c>
       <c r="AQ3" t="n">
-        <v>27.6346830136722</v>
+        <v>27.6353643727597</v>
       </c>
       <c r="AR3" t="n">
-        <v>5.89833986687364</v>
+        <v>5.89846761948121</v>
       </c>
       <c r="AS3" t="n">
-        <v>22.8000093545096</v>
+        <v>22.7983963616087</v>
       </c>
       <c r="AT3" t="n">
-        <v>6.15354258202005</v>
+        <v>6.15431759256579</v>
       </c>
       <c r="AU3" t="n">
-        <v>19.9194050531892</v>
+        <v>19.918812224541</v>
       </c>
       <c r="AV3" t="n">
-        <v>2.26045878023041</v>
+        <v>2.26042720220306</v>
       </c>
       <c r="AW3" t="n">
-        <v>4.43596692011541</v>
+        <v>4.4361168933205</v>
       </c>
       <c r="AX3" t="n">
-        <v>4.59625059561917</v>
+        <v>4.59667371642993</v>
       </c>
       <c r="AY3" t="n">
-        <v>0.952932200268358</v>
+        <v>0.953136179730074</v>
       </c>
       <c r="AZ3" t="n">
-        <v>1.97795259017601</v>
+        <v>1.97793959192075</v>
       </c>
     </row>
     <row r="4">
@@ -1089,154 +1089,154 @@
         <v>57</v>
       </c>
       <c r="C4" t="n">
-        <v>5557423</v>
+        <v>5557535</v>
       </c>
       <c r="D4" t="n">
-        <v>1228602</v>
+        <v>1228490</v>
       </c>
       <c r="E4" t="n">
-        <v>22.1074048169448</v>
+        <v>22.1049440084498</v>
       </c>
       <c r="F4" t="n">
-        <v>4328821</v>
+        <v>4329045</v>
       </c>
       <c r="G4" t="n">
-        <v>77.8925951830552</v>
+        <v>77.8950559915502</v>
       </c>
       <c r="H4" t="n">
-        <v>69562</v>
+        <v>70067</v>
       </c>
       <c r="I4" t="n">
-        <v>1.25169525515693</v>
+        <v>1.26075679235488</v>
       </c>
       <c r="J4" t="n">
-        <v>1.60695025273625</v>
+        <v>1.61853249388722</v>
       </c>
       <c r="K4" t="n">
-        <v>25515</v>
+        <v>25512</v>
       </c>
       <c r="L4" t="n">
-        <v>0.459115672857726</v>
+        <v>0.459052439615765</v>
       </c>
       <c r="M4" t="n">
-        <v>0.589421461409469</v>
+        <v>0.589321663322973</v>
       </c>
       <c r="N4" t="n">
-        <v>4233744</v>
+        <v>4233466</v>
       </c>
       <c r="O4" t="n">
-        <v>76.1817842550405</v>
+        <v>76.1752467595796</v>
       </c>
       <c r="P4" t="n">
-        <v>97.8036282858543</v>
+        <v>97.7921458427898</v>
       </c>
       <c r="Q4" t="n">
-        <v>23137</v>
+        <v>23136</v>
       </c>
       <c r="R4" t="n">
-        <v>96418</v>
+        <v>96403</v>
       </c>
       <c r="S4" t="n">
-        <v>1175064</v>
+        <v>1174972</v>
       </c>
       <c r="T4" t="n">
-        <v>136417</v>
+        <v>136414</v>
       </c>
       <c r="U4" t="n">
-        <v>943194</v>
+        <v>943122</v>
       </c>
       <c r="V4" t="n">
-        <v>312903</v>
+        <v>312881</v>
       </c>
       <c r="W4" t="n">
-        <v>897386</v>
+        <v>897349</v>
       </c>
       <c r="X4" t="n">
-        <v>77560</v>
+        <v>77566</v>
       </c>
       <c r="Y4" t="n">
-        <v>224734</v>
+        <v>224710</v>
       </c>
       <c r="Z4" t="n">
-        <v>217873</v>
+        <v>217881</v>
       </c>
       <c r="AA4" t="n">
-        <v>30593</v>
+        <v>30586</v>
       </c>
       <c r="AB4" t="n">
-        <v>98465</v>
+        <v>98446</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.416326056159483</v>
+        <v>0.416299672426714</v>
       </c>
       <c r="AD4" t="n">
-        <v>1.73494081699378</v>
+        <v>1.7346359492113</v>
       </c>
       <c r="AE4" t="n">
-        <v>21.1440446408344</v>
+        <v>21.1419631185409</v>
       </c>
       <c r="AF4" t="n">
-        <v>2.4546808835678</v>
+        <v>2.45457743406024</v>
       </c>
       <c r="AG4" t="n">
-        <v>16.971787103483</v>
+        <v>16.9701495357204</v>
       </c>
       <c r="AH4" t="n">
-        <v>5.63036141031554</v>
+        <v>5.62985208370258</v>
       </c>
       <c r="AI4" t="n">
-        <v>16.1475201725692</v>
+        <v>16.1465289917202</v>
       </c>
       <c r="AJ4" t="n">
-        <v>1.39561087935901</v>
+        <v>1.3956907153981</v>
       </c>
       <c r="AK4" t="n">
-        <v>4.04385269935364</v>
+        <v>4.04333935818668</v>
       </c>
       <c r="AL4" t="n">
-        <v>3.920396198022</v>
+        <v>3.92046113969593</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.550488958641442</v>
+        <v>0.550351909614604</v>
       </c>
       <c r="AN4" t="n">
-        <v>1.77177443574117</v>
+        <v>1.77139685130188</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.546490293225098</v>
+        <v>0.54650255842376</v>
       </c>
       <c r="AP4" t="n">
-        <v>2.2773696283951</v>
+        <v>2.27716485735329</v>
       </c>
       <c r="AQ4" t="n">
-        <v>27.7547248959786</v>
+        <v>27.7543743117342</v>
       </c>
       <c r="AR4" t="n">
-        <v>3.22213624631059</v>
+        <v>3.22227697116264</v>
       </c>
       <c r="AS4" t="n">
-        <v>22.2780120857567</v>
+        <v>22.2777742870735</v>
       </c>
       <c r="AT4" t="n">
-        <v>7.3906924934526</v>
+        <v>7.39065815102802</v>
       </c>
       <c r="AU4" t="n">
-        <v>21.1960383055754</v>
+        <v>21.1965562024119</v>
       </c>
       <c r="AV4" t="n">
-        <v>1.83194827084491</v>
+        <v>1.83221029766154</v>
       </c>
       <c r="AW4" t="n">
-        <v>5.30816223182129</v>
+        <v>5.30794389278194</v>
       </c>
       <c r="AX4" t="n">
-        <v>5.1461070863047</v>
+        <v>5.14663398737583</v>
       </c>
       <c r="AY4" t="n">
-        <v>0.722599193527053</v>
+        <v>0.722481295468063</v>
       </c>
       <c r="AZ4" t="n">
-        <v>2.32571926880794</v>
+        <v>2.3254231875253</v>
       </c>
     </row>
     <row r="5">
@@ -1247,154 +1247,154 @@
         <v>59</v>
       </c>
       <c r="C5" t="n">
-        <v>1992408</v>
+        <v>1992409</v>
       </c>
       <c r="D5" t="n">
-        <v>456672</v>
+        <v>456682</v>
       </c>
       <c r="E5" t="n">
-        <v>22.9206066227399</v>
+        <v>22.9210970237537</v>
       </c>
       <c r="F5" t="n">
-        <v>1535736</v>
+        <v>1535727</v>
       </c>
       <c r="G5" t="n">
-        <v>77.0793933772601</v>
+        <v>77.0789029762463</v>
       </c>
       <c r="H5" t="n">
-        <v>26271</v>
+        <v>26392</v>
       </c>
       <c r="I5" t="n">
-        <v>1.31855523567462</v>
+        <v>1.32462762414745</v>
       </c>
       <c r="J5" t="n">
-        <v>1.71064557970901</v>
+        <v>1.71853460934137</v>
       </c>
       <c r="K5" t="n">
-        <v>11774</v>
+        <v>11621</v>
       </c>
       <c r="L5" t="n">
-        <v>0.590943220464885</v>
+        <v>0.583263777668139</v>
       </c>
       <c r="M5" t="n">
-        <v>0.766668229435268</v>
+        <v>0.756710014214766</v>
       </c>
       <c r="N5" t="n">
-        <v>1497691</v>
+        <v>1497714</v>
       </c>
       <c r="O5" t="n">
-        <v>75.1698949211206</v>
+        <v>75.1710115744308</v>
       </c>
       <c r="P5" t="n">
-        <v>97.5226861908557</v>
+        <v>97.5247553764439</v>
       </c>
       <c r="Q5" t="n">
-        <v>10642</v>
+        <v>10643</v>
       </c>
       <c r="R5" t="n">
-        <v>33931</v>
+        <v>33932</v>
       </c>
       <c r="S5" t="n">
-        <v>394120</v>
+        <v>394119</v>
       </c>
       <c r="T5" t="n">
-        <v>49555</v>
+        <v>49557</v>
       </c>
       <c r="U5" t="n">
-        <v>409633</v>
+        <v>409643</v>
       </c>
       <c r="V5" t="n">
-        <v>107055</v>
+        <v>107057</v>
       </c>
       <c r="W5" t="n">
-        <v>277899</v>
+        <v>277901</v>
       </c>
       <c r="X5" t="n">
         <v>26543</v>
       </c>
       <c r="Y5" t="n">
-        <v>60227</v>
+        <v>60235</v>
       </c>
       <c r="Z5" t="n">
-        <v>76658</v>
+        <v>76655</v>
       </c>
       <c r="AA5" t="n">
-        <v>12737</v>
+        <v>12738</v>
       </c>
       <c r="AB5" t="n">
         <v>38691</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.534127548172864</v>
+        <v>0.534177470589623</v>
       </c>
       <c r="AD5" t="n">
-        <v>1.70301464358706</v>
+        <v>1.70306397933356</v>
       </c>
       <c r="AE5" t="n">
-        <v>19.7810890138968</v>
+        <v>19.7810288951716</v>
       </c>
       <c r="AF5" t="n">
-        <v>2.48719137847268</v>
+        <v>2.48729051113501</v>
       </c>
       <c r="AG5" t="n">
-        <v>20.5596946007043</v>
+        <v>20.5601861866715</v>
       </c>
       <c r="AH5" t="n">
-        <v>5.37314646397726</v>
+        <v>5.37324414816436</v>
       </c>
       <c r="AI5" t="n">
-        <v>13.9478962140285</v>
+        <v>13.9479895945059</v>
       </c>
       <c r="AJ5" t="n">
-        <v>1.33220705799214</v>
+        <v>1.33220638935078</v>
       </c>
       <c r="AK5" t="n">
-        <v>3.02282464234233</v>
+        <v>3.02322464915587</v>
       </c>
       <c r="AL5" t="n">
-        <v>3.84750512947147</v>
+        <v>3.84735262689538</v>
       </c>
       <c r="AM5" t="n">
-        <v>0.639276694331683</v>
+        <v>0.639326563973562</v>
       </c>
       <c r="AN5" t="n">
-        <v>1.94192153414361</v>
+        <v>1.94192055948352</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.710560456062031</v>
+        <v>0.710616312593726</v>
       </c>
       <c r="AP5" t="n">
-        <v>2.26555410962608</v>
+        <v>2.2655860865292</v>
       </c>
       <c r="AQ5" t="n">
-        <v>26.3151744919346</v>
+        <v>26.3147036082991</v>
       </c>
       <c r="AR5" t="n">
-        <v>3.30875995115147</v>
+        <v>3.30884267623859</v>
       </c>
       <c r="AS5" t="n">
-        <v>27.3509689248316</v>
+        <v>27.3512165874126</v>
       </c>
       <c r="AT5" t="n">
-        <v>7.14800315953024</v>
+        <v>7.14802692636912</v>
       </c>
       <c r="AU5" t="n">
-        <v>18.5551625802652</v>
+        <v>18.555011170357</v>
       </c>
       <c r="AV5" t="n">
-        <v>1.77226143443474</v>
+        <v>1.772234218282</v>
       </c>
       <c r="AW5" t="n">
-        <v>4.02132349062657</v>
+        <v>4.02179588359326</v>
       </c>
       <c r="AX5" t="n">
-        <v>5.11841227596347</v>
+        <v>5.11813336858706</v>
       </c>
       <c r="AY5" t="n">
-        <v>0.850442447741223</v>
+        <v>0.85049615614196</v>
       </c>
       <c r="AZ5" t="n">
-        <v>2.58337667783274</v>
+        <v>2.58333700559653</v>
       </c>
     </row>
     <row r="6">
@@ -1405,46 +1405,46 @@
         <v>61</v>
       </c>
       <c r="C6" t="n">
-        <v>2562082</v>
+        <v>2562061</v>
       </c>
       <c r="D6" t="n">
-        <v>543435</v>
+        <v>543414</v>
       </c>
       <c r="E6" t="n">
-        <v>21.210679439612</v>
+        <v>21.2100336408852</v>
       </c>
       <c r="F6" t="n">
         <v>2018647</v>
       </c>
       <c r="G6" t="n">
-        <v>78.789320560388</v>
+        <v>78.7899663591148</v>
       </c>
       <c r="H6" t="n">
-        <v>31867</v>
+        <v>31884</v>
       </c>
       <c r="I6" t="n">
-        <v>1.24379313386535</v>
+        <v>1.24446685695618</v>
       </c>
       <c r="J6" t="n">
-        <v>1.57863162801619</v>
+        <v>1.57947377624716</v>
       </c>
       <c r="K6" t="n">
-        <v>13264</v>
+        <v>13245</v>
       </c>
       <c r="L6" t="n">
-        <v>0.517703961075407</v>
+        <v>0.516966613987723</v>
       </c>
       <c r="M6" t="n">
-        <v>0.657073772680414</v>
+        <v>0.656132548186979</v>
       </c>
       <c r="N6" t="n">
-        <v>1973516</v>
+        <v>1973518</v>
       </c>
       <c r="O6" t="n">
-        <v>77.0278234654472</v>
+        <v>77.0285328881709</v>
       </c>
       <c r="P6" t="n">
-        <v>97.7642945993034</v>
+        <v>97.7643936755659</v>
       </c>
       <c r="Q6" t="n">
         <v>12965</v>
@@ -1453,7 +1453,7 @@
         <v>51193</v>
       </c>
       <c r="S6" t="n">
-        <v>647180</v>
+        <v>647172</v>
       </c>
       <c r="T6" t="n">
         <v>58653</v>
@@ -1465,94 +1465,94 @@
         <v>96984</v>
       </c>
       <c r="W6" t="n">
-        <v>407528</v>
+        <v>407527</v>
       </c>
       <c r="X6" t="n">
-        <v>43605</v>
+        <v>43596</v>
       </c>
       <c r="Y6" t="n">
         <v>122198</v>
       </c>
       <c r="Z6" t="n">
-        <v>92800</v>
+        <v>92808</v>
       </c>
       <c r="AA6" t="n">
-        <v>19914</v>
+        <v>19913</v>
       </c>
       <c r="AB6" t="n">
-        <v>35103</v>
+        <v>35116</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.50603376472728</v>
+        <v>0.506037912446269</v>
       </c>
       <c r="AD6" t="n">
-        <v>1.99810154397869</v>
+        <v>1.99811792147025</v>
       </c>
       <c r="AE6" t="n">
-        <v>25.2599253263557</v>
+        <v>25.2598201213788</v>
       </c>
       <c r="AF6" t="n">
-        <v>2.28927099132659</v>
+        <v>2.28928975539614</v>
       </c>
       <c r="AG6" t="n">
-        <v>15.0421805391084</v>
+        <v>15.0423038327347</v>
       </c>
       <c r="AH6" t="n">
-        <v>3.78535893855076</v>
+        <v>3.78538996534431</v>
       </c>
       <c r="AI6" t="n">
-        <v>15.9061263456829</v>
+        <v>15.9062176895866</v>
       </c>
       <c r="AJ6" t="n">
-        <v>1.70193615973259</v>
+        <v>1.70159883000444</v>
       </c>
       <c r="AK6" t="n">
-        <v>4.76948044598104</v>
+        <v>4.76951953915227</v>
       </c>
       <c r="AL6" t="n">
-        <v>3.62205425119102</v>
+        <v>3.6223961880689</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.777258495239419</v>
+        <v>0.777225834982071</v>
       </c>
       <c r="AN6" t="n">
-        <v>1.37009666357283</v>
+        <v>1.37061529760611</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.656949322934296</v>
+        <v>0.656948657169583</v>
       </c>
       <c r="AP6" t="n">
-        <v>2.59399974461823</v>
+        <v>2.59399711581045</v>
       </c>
       <c r="AQ6" t="n">
-        <v>32.793248192566</v>
+        <v>32.7928095918051</v>
       </c>
       <c r="AR6" t="n">
-        <v>2.97200529410453</v>
+        <v>2.97200228221886</v>
       </c>
       <c r="AS6" t="n">
-        <v>19.5282429937229</v>
+        <v>19.5282232034367</v>
       </c>
       <c r="AT6" t="n">
-        <v>4.91427482726261</v>
+        <v>4.91426984704472</v>
       </c>
       <c r="AU6" t="n">
-        <v>20.6498452508112</v>
+        <v>20.6497736529386</v>
       </c>
       <c r="AV6" t="n">
-        <v>2.20950830902815</v>
+        <v>2.20905003146665</v>
       </c>
       <c r="AW6" t="n">
-        <v>6.19189304773815</v>
+        <v>6.19188677275809</v>
       </c>
       <c r="AX6" t="n">
-        <v>4.7022674252451</v>
+        <v>4.70266802735014</v>
       </c>
       <c r="AY6" t="n">
-        <v>1.00906199899063</v>
+        <v>1.00901030545452</v>
       </c>
       <c r="AZ6" t="n">
-        <v>1.77870359297822</v>
+        <v>1.77936051254663</v>
       </c>
     </row>
     <row r="7">
@@ -1563,154 +1563,154 @@
         <v>63</v>
       </c>
       <c r="C7" t="n">
-        <v>1837324</v>
+        <v>1837328</v>
       </c>
       <c r="D7" t="n">
-        <v>459538</v>
+        <v>459528</v>
       </c>
       <c r="E7" t="n">
-        <v>25.0112663852429</v>
+        <v>25.0106676652182</v>
       </c>
       <c r="F7" t="n">
-        <v>1377786</v>
+        <v>1377800</v>
       </c>
       <c r="G7" t="n">
-        <v>74.9887336147571</v>
+        <v>74.9893323347818</v>
       </c>
       <c r="H7" t="n">
-        <v>23107</v>
+        <v>23216</v>
       </c>
       <c r="I7" t="n">
-        <v>1.25764426960079</v>
+        <v>1.26357405972151</v>
       </c>
       <c r="J7" t="n">
-        <v>1.67711095917653</v>
+        <v>1.68500508056322</v>
       </c>
       <c r="K7" t="n">
-        <v>9424</v>
+        <v>9311</v>
       </c>
       <c r="L7" t="n">
-        <v>0.512919876951479</v>
+        <v>0.506768524727213</v>
       </c>
       <c r="M7" t="n">
-        <v>0.683995918088876</v>
+        <v>0.675787487298592</v>
       </c>
       <c r="N7" t="n">
-        <v>1345255</v>
+        <v>1345273</v>
       </c>
       <c r="O7" t="n">
-        <v>73.2181694682048</v>
+        <v>73.2189897503331</v>
       </c>
       <c r="P7" t="n">
-        <v>97.6388931227346</v>
+        <v>97.6392074321382</v>
       </c>
       <c r="Q7" t="n">
         <v>9256</v>
       </c>
       <c r="R7" t="n">
-        <v>33588</v>
+        <v>33590</v>
       </c>
       <c r="S7" t="n">
-        <v>383849</v>
+        <v>383851</v>
       </c>
       <c r="T7" t="n">
-        <v>38658</v>
+        <v>38659</v>
       </c>
       <c r="U7" t="n">
-        <v>347843</v>
+        <v>347845</v>
       </c>
       <c r="V7" t="n">
         <v>88575</v>
       </c>
       <c r="W7" t="n">
-        <v>251257</v>
+        <v>251259</v>
       </c>
       <c r="X7" t="n">
-        <v>23161</v>
+        <v>23162</v>
       </c>
       <c r="Y7" t="n">
-        <v>54400</v>
+        <v>54401</v>
       </c>
       <c r="Z7" t="n">
-        <v>71689</v>
+        <v>71690</v>
       </c>
       <c r="AA7" t="n">
-        <v>11220</v>
+        <v>11226</v>
       </c>
       <c r="AB7" t="n">
         <v>31759</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.503776144000732</v>
+        <v>0.503775047242517</v>
       </c>
       <c r="AD7" t="n">
-        <v>1.82809346636739</v>
+        <v>1.82819834019838</v>
       </c>
       <c r="AE7" t="n">
-        <v>20.8917425560217</v>
+        <v>20.8918059268677</v>
       </c>
       <c r="AF7" t="n">
-        <v>2.10403826434532</v>
+        <v>2.10408811056055</v>
       </c>
       <c r="AG7" t="n">
-        <v>18.9320446475418</v>
+        <v>18.9321122847962</v>
       </c>
       <c r="AH7" t="n">
-        <v>4.8208699173363</v>
+        <v>4.82085942194317</v>
       </c>
       <c r="AI7" t="n">
-        <v>13.6751601786076</v>
+        <v>13.6752392604913</v>
       </c>
       <c r="AJ7" t="n">
-        <v>1.26058332662067</v>
+        <v>1.26063500910017</v>
       </c>
       <c r="AK7" t="n">
-        <v>2.96082781262314</v>
+        <v>2.96087579354367</v>
       </c>
       <c r="AL7" t="n">
-        <v>3.90181590182243</v>
+        <v>3.90186183414175</v>
       </c>
       <c r="AM7" t="n">
-        <v>0.610670736353523</v>
+        <v>0.610995968057962</v>
       </c>
       <c r="AN7" t="n">
-        <v>1.72854651656431</v>
+        <v>1.72854275338971</v>
       </c>
       <c r="AO7" t="n">
-        <v>0.688047990901353</v>
+        <v>0.688038784692772</v>
       </c>
       <c r="AP7" t="n">
-        <v>2.49677570423451</v>
+        <v>2.49689096562556</v>
       </c>
       <c r="AQ7" t="n">
-        <v>28.5335494014146</v>
+        <v>28.533316285988</v>
       </c>
       <c r="AR7" t="n">
-        <v>2.8736559239698</v>
+        <v>2.87369180827981</v>
       </c>
       <c r="AS7" t="n">
-        <v>25.8570308231525</v>
+        <v>25.8568335200365</v>
       </c>
       <c r="AT7" t="n">
-        <v>6.58425354300858</v>
+        <v>6.58416544448599</v>
       </c>
       <c r="AU7" t="n">
-        <v>18.6772767988225</v>
+        <v>18.677175562135</v>
       </c>
       <c r="AV7" t="n">
-        <v>1.72168101958365</v>
+        <v>1.7217323175296</v>
       </c>
       <c r="AW7" t="n">
-        <v>4.04384298887572</v>
+        <v>4.04386321586771</v>
       </c>
       <c r="AX7" t="n">
-        <v>5.32902683877778</v>
+        <v>5.32902986977364</v>
       </c>
       <c r="AY7" t="n">
-        <v>0.834042616455616</v>
+        <v>0.834477462938749</v>
       </c>
       <c r="AZ7" t="n">
-        <v>2.36081635080338</v>
+        <v>2.36078476264669</v>
       </c>
     </row>
     <row r="8">
@@ -1721,154 +1721,154 @@
         <v>65</v>
       </c>
       <c r="C8" t="n">
-        <v>7349253</v>
+        <v>7349284</v>
       </c>
       <c r="D8" t="n">
-        <v>1760731</v>
+        <v>1760727</v>
       </c>
       <c r="E8" t="n">
-        <v>23.9579587204305</v>
+        <v>23.9578032363425</v>
       </c>
       <c r="F8" t="n">
-        <v>5588522</v>
+        <v>5588557</v>
       </c>
       <c r="G8" t="n">
-        <v>76.0420412795695</v>
+        <v>76.0421967636575</v>
       </c>
       <c r="H8" t="n">
-        <v>76598</v>
+        <v>76616</v>
       </c>
       <c r="I8" t="n">
-        <v>1.04225558706443</v>
+        <v>1.04249611254647</v>
       </c>
       <c r="J8" t="n">
-        <v>1.37063073206118</v>
+        <v>1.37094423479979</v>
       </c>
       <c r="K8" t="n">
-        <v>26209</v>
+        <v>27967</v>
       </c>
       <c r="L8" t="n">
-        <v>0.356621278380265</v>
+        <v>0.380540471697651</v>
       </c>
       <c r="M8" t="n">
-        <v>0.46897909679876</v>
+        <v>0.500433296108459</v>
       </c>
       <c r="N8" t="n">
-        <v>5485715</v>
+        <v>5483974</v>
       </c>
       <c r="O8" t="n">
-        <v>74.6431644141248</v>
+        <v>74.6191601794134</v>
       </c>
       <c r="P8" t="n">
-        <v>98.1603901711401</v>
+        <v>98.1286224690918</v>
       </c>
       <c r="Q8" t="n">
-        <v>21903</v>
+        <v>21894</v>
       </c>
       <c r="R8" t="n">
-        <v>105175</v>
+        <v>105137</v>
       </c>
       <c r="S8" t="n">
-        <v>1656299</v>
+        <v>1655780</v>
       </c>
       <c r="T8" t="n">
-        <v>87361</v>
+        <v>87343</v>
       </c>
       <c r="U8" t="n">
-        <v>711720</v>
+        <v>711462</v>
       </c>
       <c r="V8" t="n">
-        <v>409481</v>
+        <v>409396</v>
       </c>
       <c r="W8" t="n">
-        <v>1659126</v>
+        <v>1658601</v>
       </c>
       <c r="X8" t="n">
-        <v>78563</v>
+        <v>78522</v>
       </c>
       <c r="Y8" t="n">
-        <v>296208</v>
+        <v>296087</v>
       </c>
       <c r="Z8" t="n">
-        <v>339459</v>
+        <v>339371</v>
       </c>
       <c r="AA8" t="n">
-        <v>33071</v>
+        <v>33050</v>
       </c>
       <c r="AB8" t="n">
-        <v>87349</v>
+        <v>87331</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.298030289609026</v>
+        <v>0.297906571578946</v>
       </c>
       <c r="AD8" t="n">
-        <v>1.43109782722135</v>
+        <v>1.43057473353867</v>
       </c>
       <c r="AE8" t="n">
-        <v>22.5369707642396</v>
+        <v>22.5298137886629</v>
       </c>
       <c r="AF8" t="n">
-        <v>1.18870584534238</v>
+        <v>1.18845590944642</v>
       </c>
       <c r="AG8" t="n">
-        <v>9.68424954209632</v>
+        <v>9.68069814692152</v>
       </c>
       <c r="AH8" t="n">
-        <v>5.57173633837344</v>
+        <v>5.57055626099087</v>
       </c>
       <c r="AI8" t="n">
-        <v>22.5754372587255</v>
+        <v>22.5681984802873</v>
       </c>
       <c r="AJ8" t="n">
-        <v>1.06899299833602</v>
+        <v>1.06843061174395</v>
       </c>
       <c r="AK8" t="n">
-        <v>4.03045044169795</v>
+        <v>4.02878702197384</v>
       </c>
       <c r="AL8" t="n">
-        <v>4.6189592329996</v>
+        <v>4.61774235422117</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.44999131204219</v>
+        <v>0.449703671813472</v>
       </c>
       <c r="AN8" t="n">
-        <v>1.18854256344148</v>
+        <v>1.18829262823426</v>
       </c>
       <c r="AO8" t="n">
-        <v>0.399273385511278</v>
+        <v>0.399236028471324</v>
       </c>
       <c r="AP8" t="n">
-        <v>1.91725235452443</v>
+        <v>1.91716809744175</v>
       </c>
       <c r="AQ8" t="n">
-        <v>30.1929465894601</v>
+        <v>30.1930680196514</v>
       </c>
       <c r="AR8" t="n">
-        <v>1.59251802180755</v>
+        <v>1.59269537018228</v>
       </c>
       <c r="AS8" t="n">
-        <v>12.9740608106692</v>
+        <v>12.9734750748271</v>
       </c>
       <c r="AT8" t="n">
-        <v>7.46449642389369</v>
+        <v>7.46531621047073</v>
       </c>
       <c r="AU8" t="n">
-        <v>30.2444804369166</v>
+        <v>30.2445088178755</v>
       </c>
       <c r="AV8" t="n">
-        <v>1.43213783435705</v>
+        <v>1.43184486286769</v>
       </c>
       <c r="AW8" t="n">
-        <v>5.39962429692392</v>
+        <v>5.39913208924769</v>
       </c>
       <c r="AX8" t="n">
-        <v>6.18805388176382</v>
+        <v>6.18841373062673</v>
       </c>
       <c r="AY8" t="n">
-        <v>0.602856692336368</v>
+        <v>0.602665147573639</v>
       </c>
       <c r="AZ8" t="n">
-        <v>1.59229927183603</v>
+        <v>1.5924765507641</v>
       </c>
     </row>
     <row r="9">
@@ -1879,154 +1879,154 @@
         <v>67</v>
       </c>
       <c r="C9" t="n">
-        <v>4323868</v>
+        <v>4323929</v>
       </c>
       <c r="D9" t="n">
-        <v>940488</v>
+        <v>940541</v>
       </c>
       <c r="E9" t="n">
-        <v>21.7510802827468</v>
+        <v>21.7519991655737</v>
       </c>
       <c r="F9" t="n">
-        <v>3383380</v>
+        <v>3383388</v>
       </c>
       <c r="G9" t="n">
-        <v>78.2489197172532</v>
+        <v>78.2480008344263</v>
       </c>
       <c r="H9" t="n">
-        <v>47631</v>
+        <v>47891</v>
       </c>
       <c r="I9" t="n">
-        <v>1.10158311955869</v>
+        <v>1.10758062863659</v>
       </c>
       <c r="J9" t="n">
-        <v>1.40779339004191</v>
+        <v>1.41547466622214</v>
       </c>
       <c r="K9" t="n">
-        <v>23690</v>
+        <v>24876</v>
       </c>
       <c r="L9" t="n">
-        <v>0.547889065993689</v>
+        <v>0.575310094129668</v>
       </c>
       <c r="M9" t="n">
-        <v>0.700187386577919</v>
+        <v>0.735239351797666</v>
       </c>
       <c r="N9" t="n">
-        <v>3312059</v>
+        <v>3310621</v>
       </c>
       <c r="O9" t="n">
-        <v>76.5994475317008</v>
+        <v>76.56511011166</v>
       </c>
       <c r="P9" t="n">
-        <v>97.8920192233802</v>
+        <v>97.8492859819802</v>
       </c>
       <c r="Q9" t="n">
-        <v>14885</v>
+        <v>14875</v>
       </c>
       <c r="R9" t="n">
-        <v>83483</v>
+        <v>83452</v>
       </c>
       <c r="S9" t="n">
-        <v>777771</v>
+        <v>777444</v>
       </c>
       <c r="T9" t="n">
-        <v>184993</v>
+        <v>184956</v>
       </c>
       <c r="U9" t="n">
-        <v>815481</v>
+        <v>815338</v>
       </c>
       <c r="V9" t="n">
-        <v>260206</v>
+        <v>260127</v>
       </c>
       <c r="W9" t="n">
-        <v>742545</v>
+        <v>741948</v>
       </c>
       <c r="X9" t="n">
-        <v>77209</v>
+        <v>77124</v>
       </c>
       <c r="Y9" t="n">
-        <v>139249</v>
+        <v>139122</v>
       </c>
       <c r="Z9" t="n">
-        <v>129083</v>
+        <v>129101</v>
       </c>
       <c r="AA9" t="n">
-        <v>23912</v>
+        <v>23891</v>
       </c>
       <c r="AB9" t="n">
-        <v>63242</v>
+        <v>63243</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.344251952187255</v>
+        <v>0.344015824496656</v>
       </c>
       <c r="AD9" t="n">
-        <v>1.93074811719507</v>
+        <v>1.93000393854756</v>
       </c>
       <c r="AE9" t="n">
-        <v>17.9878525431396</v>
+        <v>17.9800362124355</v>
       </c>
       <c r="AF9" t="n">
-        <v>4.27841460470116</v>
+        <v>4.27749854356998</v>
       </c>
       <c r="AG9" t="n">
-        <v>18.859988325268</v>
+        <v>18.8564150798961</v>
       </c>
       <c r="AH9" t="n">
-        <v>6.01789878876968</v>
+        <v>6.01598684899775</v>
       </c>
       <c r="AI9" t="n">
-        <v>17.1731653232707</v>
+        <v>17.1591161649509</v>
       </c>
       <c r="AJ9" t="n">
-        <v>1.78564655535275</v>
+        <v>1.78365555956169</v>
       </c>
       <c r="AK9" t="n">
-        <v>3.22047296540967</v>
+        <v>3.21749038894949</v>
       </c>
       <c r="AL9" t="n">
-        <v>2.98535940505122</v>
+        <v>2.98573357703145</v>
       </c>
       <c r="AM9" t="n">
-        <v>0.553023357789831</v>
+        <v>0.55252988659157</v>
       </c>
       <c r="AN9" t="n">
-        <v>1.46262559356576</v>
+        <v>1.46262808663139</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.449418322560075</v>
+        <v>0.449311473587584</v>
       </c>
       <c r="AP9" t="n">
-        <v>2.52057707909189</v>
+        <v>2.52073553571973</v>
       </c>
       <c r="AQ9" t="n">
-        <v>23.4830055865551</v>
+        <v>23.4833283544084</v>
       </c>
       <c r="AR9" t="n">
-        <v>5.58543794056809</v>
+        <v>5.58674641404135</v>
       </c>
       <c r="AS9" t="n">
-        <v>24.6215722606391</v>
+        <v>24.6279474455095</v>
       </c>
       <c r="AT9" t="n">
-        <v>7.85632140007168</v>
+        <v>7.85734760940621</v>
       </c>
       <c r="AU9" t="n">
-        <v>22.4194375764441</v>
+        <v>22.4111428037217</v>
       </c>
       <c r="AV9" t="n">
-        <v>2.33114808643204</v>
+        <v>2.32959314883824</v>
       </c>
       <c r="AW9" t="n">
-        <v>4.2043031238272</v>
+        <v>4.20229316493794</v>
       </c>
       <c r="AX9" t="n">
-        <v>3.89736414719665</v>
+        <v>3.89960070935332</v>
       </c>
       <c r="AY9" t="n">
-        <v>0.721967815186867</v>
+        <v>0.721647086755023</v>
       </c>
       <c r="AZ9" t="n">
-        <v>1.90944666142723</v>
+        <v>1.91030625372098</v>
       </c>
     </row>
     <row r="10">
@@ -2052,139 +2052,139 @@
         <v>73.0642837839426</v>
       </c>
       <c r="H10" t="n">
-        <v>42994</v>
+        <v>42945</v>
       </c>
       <c r="I10" t="n">
-        <v>1.01035167495036</v>
+        <v>1.00920018329867</v>
       </c>
       <c r="J10" t="n">
-        <v>1.38282567435829</v>
+        <v>1.38124967635755</v>
       </c>
       <c r="K10" t="n">
-        <v>21415</v>
+        <v>24270</v>
       </c>
       <c r="L10" t="n">
-        <v>0.503248851445827</v>
+        <v>0.570340865028728</v>
       </c>
       <c r="M10" t="n">
-        <v>0.688775452769752</v>
+        <v>0.780601458730884</v>
       </c>
       <c r="N10" t="n">
-        <v>3044732</v>
+        <v>3041926</v>
       </c>
       <c r="O10" t="n">
-        <v>71.5506832575464</v>
+        <v>71.4847427356152</v>
       </c>
       <c r="P10" t="n">
-        <v>97.928398872872</v>
+        <v>97.8381488649116</v>
       </c>
       <c r="Q10" t="n">
-        <v>20977</v>
+        <v>20943</v>
       </c>
       <c r="R10" t="n">
-        <v>94831</v>
+        <v>94776</v>
       </c>
       <c r="S10" t="n">
-        <v>773221</v>
+        <v>772619</v>
       </c>
       <c r="T10" t="n">
-        <v>62548</v>
+        <v>62487</v>
       </c>
       <c r="U10" t="n">
-        <v>1015361</v>
+        <v>1014182</v>
       </c>
       <c r="V10" t="n">
-        <v>179606</v>
+        <v>179416</v>
       </c>
       <c r="W10" t="n">
-        <v>577878</v>
+        <v>577487</v>
       </c>
       <c r="X10" t="n">
-        <v>40856</v>
+        <v>40814</v>
       </c>
       <c r="Y10" t="n">
-        <v>95234</v>
+        <v>95164</v>
       </c>
       <c r="Z10" t="n">
-        <v>107631</v>
+        <v>107527</v>
       </c>
       <c r="AA10" t="n">
-        <v>21150</v>
+        <v>21125</v>
       </c>
       <c r="AB10" t="n">
-        <v>55439</v>
+        <v>55386</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.492955926069536</v>
+        <v>0.492156931862244</v>
       </c>
       <c r="AD10" t="n">
-        <v>2.22851234328551</v>
+        <v>2.22721985265607</v>
       </c>
       <c r="AE10" t="n">
-        <v>18.1705617634272</v>
+        <v>18.1564148659922</v>
       </c>
       <c r="AF10" t="n">
-        <v>1.46986734346176</v>
+        <v>1.46843385385456</v>
       </c>
       <c r="AG10" t="n">
-        <v>23.8608105091238</v>
+        <v>23.8331042099945</v>
       </c>
       <c r="AH10" t="n">
-        <v>4.2207103998496</v>
+        <v>4.21624543222062</v>
       </c>
       <c r="AI10" t="n">
-        <v>13.5800345447495</v>
+        <v>13.5708461113657</v>
       </c>
       <c r="AJ10" t="n">
-        <v>0.960109039209466</v>
+        <v>0.959122046365164</v>
       </c>
       <c r="AK10" t="n">
-        <v>2.23798277462488</v>
+        <v>2.23633778655105</v>
       </c>
       <c r="AL10" t="n">
-        <v>2.52931016250132</v>
+        <v>2.52686618022019</v>
       </c>
       <c r="AM10" t="n">
-        <v>0.497021396594875</v>
+        <v>0.496433900854219</v>
       </c>
       <c r="AN10" t="n">
-        <v>1.30280705464885</v>
+        <v>1.30156156367866</v>
       </c>
       <c r="AO10" t="n">
-        <v>0.688960473368428</v>
+        <v>0.688478286454043</v>
       </c>
       <c r="AP10" t="n">
-        <v>3.11459268007825</v>
+        <v>3.11565764584674</v>
       </c>
       <c r="AQ10" t="n">
-        <v>25.3953714152838</v>
+        <v>25.3990070764378</v>
       </c>
       <c r="AR10" t="n">
-        <v>2.05430231626297</v>
+        <v>2.05419198231647</v>
       </c>
       <c r="AS10" t="n">
-        <v>33.3481239071288</v>
+        <v>33.340127274628</v>
       </c>
       <c r="AT10" t="n">
-        <v>5.89890998616627</v>
+        <v>5.89810534510044</v>
       </c>
       <c r="AU10" t="n">
-        <v>18.9796014887353</v>
+        <v>18.9842553697887</v>
       </c>
       <c r="AV10" t="n">
-        <v>1.34185865948136</v>
+        <v>1.34171574193455</v>
       </c>
       <c r="AW10" t="n">
-        <v>3.12782865618386</v>
+        <v>3.12841272272895</v>
       </c>
       <c r="AX10" t="n">
-        <v>3.53499092859404</v>
+        <v>3.53483286575676</v>
       </c>
       <c r="AY10" t="n">
-        <v>0.694642418446024</v>
+        <v>0.694461337981266</v>
       </c>
       <c r="AZ10" t="n">
-        <v>1.82081707027088</v>
+        <v>1.82075435102629</v>
       </c>
     </row>
     <row r="11">
@@ -2195,46 +2195,46 @@
         <v>71</v>
       </c>
       <c r="C11" t="n">
-        <v>2413801</v>
+        <v>2413749</v>
       </c>
       <c r="D11" t="n">
-        <v>590836</v>
+        <v>590804</v>
       </c>
       <c r="E11" t="n">
-        <v>24.4774113524686</v>
+        <v>24.4766129369707</v>
       </c>
       <c r="F11" t="n">
-        <v>1822965</v>
+        <v>1822945</v>
       </c>
       <c r="G11" t="n">
-        <v>75.5225886475314</v>
+        <v>75.5233870630293</v>
       </c>
       <c r="H11" t="n">
-        <v>28659</v>
+        <v>28947</v>
       </c>
       <c r="I11" t="n">
-        <v>1.18729754441232</v>
+        <v>1.19925476924071</v>
       </c>
       <c r="J11" t="n">
-        <v>1.57210917379105</v>
+        <v>1.58792503339377</v>
       </c>
       <c r="K11" t="n">
-        <v>10852</v>
+        <v>10533</v>
       </c>
       <c r="L11" t="n">
-        <v>0.449581386369465</v>
+        <v>0.436375116053906</v>
       </c>
       <c r="M11" t="n">
-        <v>0.595293930492357</v>
+        <v>0.577801305031145</v>
       </c>
       <c r="N11" t="n">
-        <v>1783454</v>
+        <v>1783465</v>
       </c>
       <c r="O11" t="n">
-        <v>73.8857097167496</v>
+        <v>73.8877571777347</v>
       </c>
       <c r="P11" t="n">
-        <v>97.8325968957166</v>
+        <v>97.8342736615751</v>
       </c>
       <c r="Q11" t="n">
         <v>12839</v>
@@ -2243,106 +2243,106 @@
         <v>46358</v>
       </c>
       <c r="S11" t="n">
-        <v>521761</v>
+        <v>521769</v>
       </c>
       <c r="T11" t="n">
-        <v>45487</v>
+        <v>45488</v>
       </c>
       <c r="U11" t="n">
-        <v>484096</v>
+        <v>484106</v>
       </c>
       <c r="V11" t="n">
         <v>99446</v>
       </c>
       <c r="W11" t="n">
-        <v>335582</v>
+        <v>335590</v>
       </c>
       <c r="X11" t="n">
-        <v>30234</v>
+        <v>30235</v>
       </c>
       <c r="Y11" t="n">
-        <v>73288</v>
+        <v>73269</v>
       </c>
       <c r="Z11" t="n">
-        <v>79799</v>
+        <v>79800</v>
       </c>
       <c r="AA11" t="n">
         <v>16005</v>
       </c>
       <c r="AB11" t="n">
-        <v>38559</v>
+        <v>38560</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.53189968849959</v>
+        <v>0.531911147347964</v>
       </c>
       <c r="AD11" t="n">
-        <v>1.92053943137815</v>
+        <v>1.92058080604073</v>
       </c>
       <c r="AE11" t="n">
-        <v>21.6157421427864</v>
+        <v>21.6165392507672</v>
       </c>
       <c r="AF11" t="n">
-        <v>1.88445526371064</v>
+        <v>1.88453729033135</v>
       </c>
       <c r="AG11" t="n">
-        <v>20.0553401046731</v>
+        <v>20.0561864551782</v>
       </c>
       <c r="AH11" t="n">
-        <v>4.11989223635254</v>
+        <v>4.11998099222413</v>
       </c>
       <c r="AI11" t="n">
-        <v>13.9026373756577</v>
+        <v>13.9032683182883</v>
       </c>
       <c r="AJ11" t="n">
-        <v>1.2525473309523</v>
+        <v>1.25261574422196</v>
       </c>
       <c r="AK11" t="n">
-        <v>3.03620721012213</v>
+        <v>3.03548546265581</v>
       </c>
       <c r="AL11" t="n">
-        <v>3.30594775625663</v>
+        <v>3.30606040644657</v>
       </c>
       <c r="AM11" t="n">
-        <v>0.663062116553933</v>
+        <v>0.663076401067385</v>
       </c>
       <c r="AN11" t="n">
-        <v>1.5974390598065</v>
+        <v>1.59751490316516</v>
       </c>
       <c r="AO11" t="n">
-        <v>0.71989521456679</v>
+        <v>0.719890774419459</v>
       </c>
       <c r="AP11" t="n">
-        <v>2.59933813824186</v>
+        <v>2.59932210612488</v>
       </c>
       <c r="AQ11" t="n">
-        <v>29.2556466272749</v>
+        <v>29.2559147502194</v>
       </c>
       <c r="AR11" t="n">
-        <v>2.55050032128667</v>
+        <v>2.55054066101662</v>
       </c>
       <c r="AS11" t="n">
-        <v>27.1437334520543</v>
+        <v>27.1441267420443</v>
       </c>
       <c r="AT11" t="n">
-        <v>5.57603392069546</v>
+        <v>5.57599952900674</v>
       </c>
       <c r="AU11" t="n">
-        <v>18.8164090579292</v>
+        <v>18.8167415676786</v>
       </c>
       <c r="AV11" t="n">
-        <v>1.69524977936072</v>
+        <v>1.69529539407838</v>
       </c>
       <c r="AW11" t="n">
-        <v>4.10932942481275</v>
+        <v>4.10823873751377</v>
       </c>
       <c r="AX11" t="n">
-        <v>4.4744075260702</v>
+        <v>4.47443599958508</v>
       </c>
       <c r="AY11" t="n">
-        <v>0.897415913166249</v>
+        <v>0.89741037811227</v>
       </c>
       <c r="AZ11" t="n">
-        <v>2.16204062454092</v>
+        <v>2.16208336020051</v>
       </c>
     </row>
     <row r="12">
@@ -2353,154 +2353,154 @@
         <v>73</v>
       </c>
       <c r="C12" t="n">
-        <v>2832899</v>
+        <v>2832949</v>
       </c>
       <c r="D12" t="n">
-        <v>652103</v>
+        <v>652018</v>
       </c>
       <c r="E12" t="n">
-        <v>23.0189286663591</v>
+        <v>23.0155219878649</v>
       </c>
       <c r="F12" t="n">
-        <v>2180796</v>
+        <v>2180931</v>
       </c>
       <c r="G12" t="n">
-        <v>76.9810713336409</v>
+        <v>76.9844780121351</v>
       </c>
       <c r="H12" t="n">
-        <v>38855</v>
+        <v>38934</v>
       </c>
       <c r="I12" t="n">
-        <v>1.37156319374605</v>
+        <v>1.37432759996738</v>
       </c>
       <c r="J12" t="n">
-        <v>1.78168888791065</v>
+        <v>1.78520090731894</v>
       </c>
       <c r="K12" t="n">
-        <v>14622</v>
+        <v>14554</v>
       </c>
       <c r="L12" t="n">
-        <v>0.516149710949808</v>
+        <v>0.513740275592677</v>
       </c>
       <c r="M12" t="n">
-        <v>0.670489124154666</v>
+        <v>0.667329686267012</v>
       </c>
       <c r="N12" t="n">
-        <v>2127319</v>
+        <v>2127443</v>
       </c>
       <c r="O12" t="n">
-        <v>75.093358428945</v>
+        <v>75.096410136575</v>
       </c>
       <c r="P12" t="n">
-        <v>97.5478219879347</v>
+        <v>97.547469406414</v>
       </c>
       <c r="Q12" t="n">
-        <v>13861</v>
+        <v>13853</v>
       </c>
       <c r="R12" t="n">
-        <v>45056</v>
+        <v>45058</v>
       </c>
       <c r="S12" t="n">
-        <v>707913</v>
+        <v>707890</v>
       </c>
       <c r="T12" t="n">
-        <v>54584</v>
+        <v>54592</v>
       </c>
       <c r="U12" t="n">
-        <v>441979</v>
+        <v>442025</v>
       </c>
       <c r="V12" t="n">
-        <v>114377</v>
+        <v>114388</v>
       </c>
       <c r="W12" t="n">
-        <v>408959</v>
+        <v>408969</v>
       </c>
       <c r="X12" t="n">
-        <v>43286</v>
+        <v>43291</v>
       </c>
       <c r="Y12" t="n">
-        <v>127892</v>
+        <v>127935</v>
       </c>
       <c r="Z12" t="n">
-        <v>106769</v>
+        <v>106786</v>
       </c>
       <c r="AA12" t="n">
-        <v>18431</v>
+        <v>18441</v>
       </c>
       <c r="AB12" t="n">
-        <v>44212</v>
+        <v>44215</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.489286769489488</v>
+        <v>0.488995742598967</v>
       </c>
       <c r="AD12" t="n">
-        <v>1.59045557218948</v>
+        <v>1.59049809933041</v>
       </c>
       <c r="AE12" t="n">
-        <v>24.9889953718788</v>
+        <v>24.9877424549471</v>
       </c>
       <c r="AF12" t="n">
-        <v>1.92678948314077</v>
+        <v>1.92703786760722</v>
       </c>
       <c r="AG12" t="n">
-        <v>15.6016504647712</v>
+        <v>15.6029988538445</v>
       </c>
       <c r="AH12" t="n">
-        <v>4.03745421209863</v>
+        <v>4.03777124120484</v>
       </c>
       <c r="AI12" t="n">
-        <v>14.4360600219069</v>
+        <v>14.4361582224036</v>
       </c>
       <c r="AJ12" t="n">
-        <v>1.52797540611225</v>
+        <v>1.52812493271146</v>
       </c>
       <c r="AK12" t="n">
-        <v>4.51452734460353</v>
+        <v>4.51596551861682</v>
       </c>
       <c r="AL12" t="n">
-        <v>3.76889539655314</v>
+        <v>3.76942895901056</v>
       </c>
       <c r="AM12" t="n">
-        <v>0.650605616366838</v>
+        <v>0.650947122592041</v>
       </c>
       <c r="AN12" t="n">
-        <v>1.56066276983401</v>
+        <v>1.56074112170745</v>
       </c>
       <c r="AO12" t="n">
-        <v>0.651571297017514</v>
+        <v>0.651157281299663</v>
       </c>
       <c r="AP12" t="n">
-        <v>2.11797102362175</v>
+        <v>2.11794158527396</v>
       </c>
       <c r="AQ12" t="n">
-        <v>33.2772376874366</v>
+        <v>33.2742169825467</v>
       </c>
       <c r="AR12" t="n">
-        <v>2.56585871700483</v>
+        <v>2.56608520181269</v>
       </c>
       <c r="AS12" t="n">
-        <v>20.7763386685307</v>
+        <v>20.777289920341</v>
       </c>
       <c r="AT12" t="n">
-        <v>5.37657962910123</v>
+        <v>5.37678330277239</v>
       </c>
       <c r="AU12" t="n">
-        <v>19.2241502097241</v>
+        <v>19.2234997600406</v>
       </c>
       <c r="AV12" t="n">
-        <v>2.03476770526658</v>
+        <v>2.03488413085568</v>
       </c>
       <c r="AW12" t="n">
-        <v>6.01188632264367</v>
+        <v>6.01355711997924</v>
       </c>
       <c r="AX12" t="n">
-        <v>5.01894638274749</v>
+        <v>5.01945293011376</v>
       </c>
       <c r="AY12" t="n">
-        <v>0.866395683957131</v>
+        <v>0.86681523312258</v>
       </c>
       <c r="AZ12" t="n">
-        <v>2.07829667294844</v>
+        <v>2.07831655184181</v>
       </c>
     </row>
     <row r="13">
@@ -2511,154 +2511,154 @@
         <v>75</v>
       </c>
       <c r="C13" t="n">
-        <v>3663891</v>
+        <v>3663871</v>
       </c>
       <c r="D13" t="n">
-        <v>959596</v>
+        <v>959575</v>
       </c>
       <c r="E13" t="n">
-        <v>26.1906263041122</v>
+        <v>26.1901961067952</v>
       </c>
       <c r="F13" t="n">
-        <v>2704295</v>
+        <v>2704296</v>
       </c>
       <c r="G13" t="n">
-        <v>73.8093736958878</v>
+        <v>73.8098038932047</v>
       </c>
       <c r="H13" t="n">
-        <v>35867</v>
+        <v>35917</v>
       </c>
       <c r="I13" t="n">
-        <v>0.978931960585072</v>
+        <v>0.980301981155996</v>
       </c>
       <c r="J13" t="n">
-        <v>1.32629761176203</v>
+        <v>1.3281460313516</v>
       </c>
       <c r="K13" t="n">
-        <v>14214</v>
+        <v>15471</v>
       </c>
       <c r="L13" t="n">
-        <v>0.387948222258795</v>
+        <v>0.422258316409066</v>
       </c>
       <c r="M13" t="n">
-        <v>0.525608337847757</v>
+        <v>0.572089741655499</v>
       </c>
       <c r="N13" t="n">
-        <v>2654214</v>
+        <v>2652908</v>
       </c>
       <c r="O13" t="n">
-        <v>72.4424935130439</v>
+        <v>72.4072435956397</v>
       </c>
       <c r="P13" t="n">
-        <v>98.1480940503902</v>
+        <v>98.0997642269929</v>
       </c>
       <c r="Q13" t="n">
-        <v>9473</v>
+        <v>9457</v>
       </c>
       <c r="R13" t="n">
-        <v>54730</v>
+        <v>54718</v>
       </c>
       <c r="S13" t="n">
-        <v>619529</v>
+        <v>619272</v>
       </c>
       <c r="T13" t="n">
-        <v>72847</v>
+        <v>72830</v>
       </c>
       <c r="U13" t="n">
-        <v>732376</v>
+        <v>732078</v>
       </c>
       <c r="V13" t="n">
-        <v>310837</v>
+        <v>310717</v>
       </c>
       <c r="W13" t="n">
-        <v>524676</v>
+        <v>524211</v>
       </c>
       <c r="X13" t="n">
-        <v>29511</v>
+        <v>29501</v>
       </c>
       <c r="Y13" t="n">
-        <v>107670</v>
+        <v>107625</v>
       </c>
       <c r="Z13" t="n">
-        <v>116137</v>
+        <v>116094</v>
       </c>
       <c r="AA13" t="n">
-        <v>16224</v>
+        <v>16219</v>
       </c>
       <c r="AB13" t="n">
-        <v>60204</v>
+        <v>60186</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.258550268007427</v>
+        <v>0.258114982760037</v>
       </c>
       <c r="AD13" t="n">
-        <v>1.49376714536541</v>
+        <v>1.49344777695503</v>
       </c>
       <c r="AE13" t="n">
-        <v>16.9090456020662</v>
+        <v>16.9021234644997</v>
       </c>
       <c r="AF13" t="n">
-        <v>1.98824146242342</v>
+        <v>1.98778832551692</v>
       </c>
       <c r="AG13" t="n">
-        <v>19.9890225991985</v>
+        <v>19.9809982392939</v>
       </c>
       <c r="AH13" t="n">
-        <v>8.48379496005749</v>
+        <v>8.4805660461299</v>
       </c>
       <c r="AI13" t="n">
-        <v>14.3201858352227</v>
+        <v>14.3075725100583</v>
       </c>
       <c r="AJ13" t="n">
-        <v>0.805455184119833</v>
+        <v>0.805186645490521</v>
       </c>
       <c r="AK13" t="n">
-        <v>2.93867912555259</v>
+        <v>2.93746695776134</v>
       </c>
       <c r="AL13" t="n">
-        <v>3.16977224486209</v>
+        <v>3.16861592561528</v>
       </c>
       <c r="AM13" t="n">
-        <v>0.442807932877916</v>
+        <v>0.442673882350115</v>
       </c>
       <c r="AN13" t="n">
-        <v>1.64317115329031</v>
+        <v>1.64268883920859</v>
       </c>
       <c r="AO13" t="n">
-        <v>0.356904153169262</v>
+        <v>0.356476741749054</v>
       </c>
       <c r="AP13" t="n">
-        <v>2.06200404338158</v>
+        <v>2.06256681347412</v>
       </c>
       <c r="AQ13" t="n">
-        <v>23.3413357023963</v>
+        <v>23.343138925285</v>
       </c>
       <c r="AR13" t="n">
-        <v>2.74457899777486</v>
+        <v>2.74528932024782</v>
       </c>
       <c r="AS13" t="n">
-        <v>27.5929521884822</v>
+        <v>27.5953029656513</v>
       </c>
       <c r="AT13" t="n">
-        <v>11.7110752938535</v>
+        <v>11.7123172005965</v>
       </c>
       <c r="AU13" t="n">
-        <v>19.7676600304271</v>
+        <v>19.7598635158098</v>
       </c>
       <c r="AV13" t="n">
-        <v>1.11185458293868</v>
+        <v>1.11202499295113</v>
       </c>
       <c r="AW13" t="n">
-        <v>4.05656815916124</v>
+        <v>4.05686891516781</v>
       </c>
       <c r="AX13" t="n">
-        <v>4.37557031949948</v>
+        <v>4.37610350603941</v>
       </c>
       <c r="AY13" t="n">
-        <v>0.611254405258958</v>
+        <v>0.611366847248378</v>
       </c>
       <c r="AZ13" t="n">
-        <v>2.26824212365695</v>
+        <v>2.2686802557797</v>
       </c>
     </row>
     <row r="14">
@@ -2669,154 +2669,154 @@
         <v>77</v>
       </c>
       <c r="C14" t="n">
-        <v>243049</v>
+        <v>243032</v>
       </c>
       <c r="D14" t="n">
-        <v>90643</v>
+        <v>90629</v>
       </c>
       <c r="E14" t="n">
-        <v>37.2941258758522</v>
+        <v>37.2909740281115</v>
       </c>
       <c r="F14" t="n">
-        <v>152406</v>
+        <v>152403</v>
       </c>
       <c r="G14" t="n">
-        <v>62.7058741241478</v>
+        <v>62.7090259718885</v>
       </c>
       <c r="H14" t="n">
-        <v>2475</v>
+        <v>2593</v>
       </c>
       <c r="I14" t="n">
-        <v>1.0183131796469</v>
+        <v>1.06693768721814</v>
       </c>
       <c r="J14" t="n">
-        <v>1.62395181292075</v>
+        <v>1.70141007722945</v>
       </c>
       <c r="K14" t="n">
-        <v>1994</v>
+        <v>2438</v>
       </c>
       <c r="L14" t="n">
-        <v>0.820410699077141</v>
+        <v>1.00316007768524</v>
       </c>
       <c r="M14" t="n">
-        <v>1.30834744038949</v>
+        <v>1.59970604253197</v>
       </c>
       <c r="N14" t="n">
-        <v>147937</v>
+        <v>147372</v>
       </c>
       <c r="O14" t="n">
-        <v>60.8671502454238</v>
+        <v>60.6389282069851</v>
       </c>
       <c r="P14" t="n">
-        <v>97.0677007466898</v>
+        <v>96.6988838802386</v>
       </c>
       <c r="Q14" t="n">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="R14" t="n">
-        <v>4553</v>
+        <v>4537</v>
       </c>
       <c r="S14" t="n">
-        <v>26794</v>
+        <v>26705</v>
       </c>
       <c r="T14" t="n">
-        <v>15408</v>
+        <v>15330</v>
       </c>
       <c r="U14" t="n">
-        <v>42284</v>
+        <v>42137</v>
       </c>
       <c r="V14" t="n">
-        <v>18936</v>
+        <v>18856</v>
       </c>
       <c r="W14" t="n">
-        <v>19779</v>
+        <v>19698</v>
       </c>
       <c r="X14" t="n">
-        <v>1592</v>
+        <v>1583</v>
       </c>
       <c r="Y14" t="n">
-        <v>4801</v>
+        <v>4786</v>
       </c>
       <c r="Z14" t="n">
-        <v>9360</v>
+        <v>9327</v>
       </c>
       <c r="AA14" t="n">
-        <v>1374</v>
+        <v>1370</v>
       </c>
       <c r="AB14" t="n">
-        <v>2601</v>
+        <v>2589</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.187205049187612</v>
+        <v>0.18680667566411</v>
       </c>
       <c r="AD14" t="n">
-        <v>1.87328481088176</v>
+        <v>1.8668323512953</v>
       </c>
       <c r="AE14" t="n">
-        <v>11.0241144789734</v>
+        <v>10.9882649198459</v>
       </c>
       <c r="AF14" t="n">
-        <v>6.33946241292908</v>
+        <v>6.30781131702821</v>
       </c>
       <c r="AG14" t="n">
-        <v>17.3973149447231</v>
+        <v>17.3380460186313</v>
       </c>
       <c r="AH14" t="n">
-        <v>7.79102156355303</v>
+        <v>7.75864906678956</v>
       </c>
       <c r="AI14" t="n">
-        <v>8.13786520413579</v>
+        <v>8.10510550051022</v>
       </c>
       <c r="AJ14" t="n">
-        <v>0.655011952322371</v>
+        <v>0.651354554132789</v>
       </c>
       <c r="AK14" t="n">
-        <v>1.97532184868072</v>
+        <v>1.96928799499654</v>
       </c>
       <c r="AL14" t="n">
-        <v>3.85107529757374</v>
+        <v>3.83776622008624</v>
       </c>
       <c r="AM14" t="n">
-        <v>0.565318104579735</v>
+        <v>0.563711774581125</v>
       </c>
       <c r="AN14" t="n">
-        <v>1.07015457788347</v>
+        <v>1.06529181342375</v>
       </c>
       <c r="AO14" t="n">
-        <v>0.307563354671245</v>
+        <v>0.30806394701843</v>
       </c>
       <c r="AP14" t="n">
-        <v>3.07766143696303</v>
+        <v>3.07860380533616</v>
       </c>
       <c r="AQ14" t="n">
-        <v>18.1117637913436</v>
+        <v>18.1208099231876</v>
       </c>
       <c r="AR14" t="n">
-        <v>10.415244326977</v>
+        <v>10.4022473739923</v>
       </c>
       <c r="AS14" t="n">
-        <v>28.5824371185031</v>
+        <v>28.5922699020167</v>
       </c>
       <c r="AT14" t="n">
-        <v>12.8000432616587</v>
+        <v>12.7948321255055</v>
       </c>
       <c r="AU14" t="n">
-        <v>13.3698804220716</v>
+        <v>13.3661753928833</v>
       </c>
       <c r="AV14" t="n">
-        <v>1.07613375964093</v>
+        <v>1.07415248486822</v>
       </c>
       <c r="AW14" t="n">
-        <v>3.24530036434428</v>
+        <v>3.24756398773173</v>
       </c>
       <c r="AX14" t="n">
-        <v>6.32701758180847</v>
+        <v>6.3288820128654</v>
       </c>
       <c r="AY14" t="n">
-        <v>0.928773734765474</v>
+        <v>0.929620280650327</v>
       </c>
       <c r="AZ14" t="n">
-        <v>1.75818084725255</v>
+        <v>1.7567787639443</v>
       </c>
     </row>
     <row r="15">
@@ -3316,22 +3316,22 @@
         <v>53.6430909244322</v>
       </c>
       <c r="H18" t="n">
-        <v>7359</v>
+        <v>7361</v>
       </c>
       <c r="I18" t="n">
-        <v>1.08935235419421</v>
+        <v>1.0896484140812</v>
       </c>
       <c r="J18" t="n">
-        <v>2.0307412108836</v>
+        <v>2.03129311772173</v>
       </c>
       <c r="K18" t="n">
-        <v>8255</v>
+        <v>8253</v>
       </c>
       <c r="L18" t="n">
-        <v>1.22198718356749</v>
+        <v>1.2216911236805</v>
       </c>
       <c r="M18" t="n">
-        <v>2.27799547436393</v>
+        <v>2.2774435675258</v>
       </c>
       <c r="N18" t="n">
         <v>346766</v>
@@ -3462,43 +3462,43 @@
         <v>92187</v>
       </c>
       <c r="D19" t="n">
-        <v>55023</v>
+        <v>55024</v>
       </c>
       <c r="E19" t="n">
-        <v>59.6862898239448</v>
+        <v>59.6873745755909</v>
       </c>
       <c r="F19" t="n">
-        <v>37164</v>
+        <v>37163</v>
       </c>
       <c r="G19" t="n">
-        <v>40.3137101760552</v>
+        <v>40.3126254244091</v>
       </c>
       <c r="H19" t="n">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="I19" t="n">
-        <v>1.0012257693601</v>
+        <v>1.00014101771399</v>
       </c>
       <c r="J19" t="n">
-        <v>2.48358626627919</v>
+        <v>2.4809622473966</v>
       </c>
       <c r="K19" t="n">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="L19" t="n">
-        <v>1.29085445887164</v>
+        <v>1.29193921051775</v>
       </c>
       <c r="M19" t="n">
-        <v>3.20202346356689</v>
+        <v>3.20480047358932</v>
       </c>
       <c r="N19" t="n">
-        <v>35051</v>
+        <v>35050</v>
       </c>
       <c r="O19" t="n">
-        <v>38.0216299478234</v>
+        <v>38.0205451961773</v>
       </c>
       <c r="P19" t="n">
-        <v>94.3143902701539</v>
+        <v>94.3142372790141</v>
       </c>
       <c r="Q19" t="n">
         <v>430</v>
@@ -3519,7 +3519,7 @@
         <v>482</v>
       </c>
       <c r="W19" t="n">
-        <v>8399</v>
+        <v>8398</v>
       </c>
       <c r="X19" t="n">
         <v>318</v>
@@ -3555,7 +3555,7 @@
         <v>0.52285029342532</v>
       </c>
       <c r="AI19" t="n">
-        <v>9.11082907568312</v>
+        <v>9.10974432403701</v>
       </c>
       <c r="AJ19" t="n">
         <v>0.344951023463178</v>
@@ -3573,40 +3573,40 @@
         <v>0.57491837243863</v>
       </c>
       <c r="AO19" t="n">
-        <v>1.22678382927734</v>
+        <v>1.22681883024251</v>
       </c>
       <c r="AP19" t="n">
-        <v>0.58771504379333</v>
+        <v>0.587731811697575</v>
       </c>
       <c r="AQ19" t="n">
-        <v>16.9353228153262</v>
+        <v>16.9358059914408</v>
       </c>
       <c r="AR19" t="n">
-        <v>1.0242218481641</v>
+        <v>1.02425106990014</v>
       </c>
       <c r="AS19" t="n">
-        <v>42.6749593449545</v>
+        <v>42.6761768901569</v>
       </c>
       <c r="AT19" t="n">
-        <v>1.37513908305041</v>
+        <v>1.37517831669044</v>
       </c>
       <c r="AU19" t="n">
-        <v>23.9622264700009</v>
+        <v>23.9600570613409</v>
       </c>
       <c r="AV19" t="n">
-        <v>0.907249436535334</v>
+        <v>0.907275320970043</v>
       </c>
       <c r="AW19" t="n">
-        <v>0.841630766597244</v>
+        <v>0.841654778887304</v>
       </c>
       <c r="AX19" t="n">
-        <v>8.01688967504493</v>
+        <v>8.01711840228245</v>
       </c>
       <c r="AY19" t="n">
-        <v>0.935779293030156</v>
+        <v>0.935805991440799</v>
       </c>
       <c r="AZ19" t="n">
-        <v>1.51208239422556</v>
+        <v>1.51212553495007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>